<commit_message>
Atualização automática de SAO_FRANCISCO_DE_ASSIS.xlsx
</commit_message>
<xml_diff>
--- a/SAO_FRANCISCO_DE_ASSIS.xlsx
+++ b/SAO_FRANCISCO_DE_ASSIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F87496D-21F4-446C-B186-453EE5F12120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61304848-EFCE-4414-9EBE-5285C74DBA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1204,7 +1204,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{1F22E988-7900-4994-B3B0-8350C3D07EEC}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{825649A7-43D5-494F-999B-364D5ACF7D1C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1234,10 +1234,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC8BC0A-6B54-40BC-8C62-EFED456F2B66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D8379C4-CF8A-4ADF-ABAA-AC5028591CF4}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1275,7 +1275,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8211ECBA-62B1-4837-848F-C0CE7B7049EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63C71972-6E76-4B91-8FB4-913FA363E76B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1338,7 +1338,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95A09DCC-21C2-49C8-AF3E-E6E7AA5B5571}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79EB9845-830C-4CE7-B23C-C5B3821DDC4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1357,7 +1357,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2E6C929-BD4C-7370-05D8-E387D1D78A6A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73929150-DD10-ECB3-3BA8-A610576556EC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1406,7 +1406,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2875DB3F-8A64-5AE5-FCEF-F996126F163C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{256CFB98-79FD-55D0-85D8-8860D28B1CA0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1425,7 +1425,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{177B07DA-EC72-807C-E92F-E3373A8EA1B1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD737897-8755-23FA-B43F-799E020AFEA6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1456,7 +1456,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0961F89-FCD0-0593-B6C0-D56D505758EC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93D3165C-4B53-0DBA-D4F1-DB0EB3EEB41C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1487,7 +1487,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7951A3C7-369D-AC4E-E674-D5344650B23A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA582DB3-1EF0-AA37-BAA4-4725BFDC4AFB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1530,7 +1530,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C0EC9AA-BE1F-496A-8CFF-1B069D8AF413}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48CC2DAE-4535-4C4D-BA4F-55430613FBD5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1568,7 +1568,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{149A612B-C247-4E8C-9E3D-6A7F556D404A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92A02279-B29A-407D-A584-A0FA6966F18A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1611,7 +1611,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4900300-1EBD-4CBB-9878-4301F163797B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11D3E6E6-9514-4F85-8BE0-818D69ADE9FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1924,7 +1924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2EDC35-C8C6-44F0-8D09-E16A6A713225}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78AEA2CC-6CA8-475C-B0CC-C4B560CFA8A5}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>